<commit_message>
data till 3Feb 10AM
</commit_message>
<xml_diff>
--- a/Daily Collection/February-2021-Collection.xlsx
+++ b/Daily Collection/February-2021-Collection.xlsx
@@ -45,6 +45,29 @@
         </r>
       </text>
     </comment>
+    <comment ref="H48" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>Vijay:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+2000-Cash
+2000-Digital</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G53" authorId="0">
       <text>
         <r>
@@ -556,8 +579,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -579,7 +602,14 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -587,7 +617,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -601,9 +639,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -616,7 +684,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -626,37 +694,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -676,15 +713,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,35 +737,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -765,7 +788,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,73 +938,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,97 +968,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -956,6 +979,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1016,6 +1054,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1030,38 +1079,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1079,130 +1102,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1591,11 +1614,11 @@
   <dimension ref="A1:AO110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G78" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I48" sqref="I48"/>
+      <selection pane="bottomRight" activeCell="H96" sqref="H96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1726,14 +1749,14 @@
       <c r="C2" s="7"/>
       <c r="D2" s="8">
         <f>SUM(F3:F121)</f>
-        <v>58700</v>
+        <v>95900</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="8">
         <f>SUM(G2:AK2)</f>
-        <v>58700</v>
+        <v>95900</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G121)</f>
@@ -1741,7 +1764,7 @@
       </c>
       <c r="H2" s="2">
         <f>SUM(H3:H121)</f>
-        <v>0</v>
+        <v>37200</v>
       </c>
       <c r="I2" s="2">
         <f>SUM(I3:I121)</f>
@@ -2367,10 +2390,12 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4">
+        <v>1500</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -2476,12 +2501,14 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>4500</v>
+        <v>6500</v>
       </c>
       <c r="G14" s="4">
         <v>4500</v>
       </c>
-      <c r="H14" s="4"/>
+      <c r="H14" s="4">
+        <v>2000</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
@@ -2648,10 +2675,12 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="4">
+        <v>1000</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
@@ -2813,10 +2842,12 @@
       </c>
       <c r="F20" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="4">
+        <v>1000</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -3252,12 +3283,14 @@
       </c>
       <c r="F28" s="1">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G28" s="4">
         <v>1000</v>
       </c>
-      <c r="H28" s="4"/>
+      <c r="H28" s="4">
+        <v>1000</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -3307,10 +3340,12 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5500</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
+      <c r="H29" s="4">
+        <v>5500</v>
+      </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -3620,10 +3655,12 @@
       </c>
       <c r="F35" s="1">
         <f t="shared" ref="F35:F67" si="2">SUM(G35:AK35)</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
+      <c r="H35" s="11">
+        <v>3000</v>
+      </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
@@ -3934,10 +3971,12 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
+      <c r="H41" s="4">
+        <v>1500</v>
+      </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -4137,10 +4176,12 @@
       </c>
       <c r="F45" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="4"/>
+      <c r="H45" s="4">
+        <v>3000</v>
+      </c>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
@@ -4296,10 +4337,12 @@
       </c>
       <c r="F48" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
+      <c r="H48" s="11">
+        <v>4000</v>
+      </c>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
@@ -4666,10 +4709,12 @@
       </c>
       <c r="F55" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
+      <c r="H55" s="4">
+        <v>2000</v>
+      </c>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
@@ -4769,10 +4814,12 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
+      <c r="H57" s="4">
+        <v>2000</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -4988,10 +5035,12 @@
       </c>
       <c r="F61" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
+      <c r="H61" s="4">
+        <v>1500</v>
+      </c>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -5454,10 +5503,12 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
+      <c r="H70" s="4">
+        <v>1200</v>
+      </c>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
@@ -6559,10 +6610,12 @@
       </c>
       <c r="F92" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="G92" s="4"/>
-      <c r="H92" s="4"/>
+      <c r="H92" s="4">
+        <v>5000</v>
+      </c>
       <c r="I92" s="4"/>
       <c r="J92" s="4"/>
       <c r="K92" s="4"/>
@@ -6762,10 +6815,12 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G96" s="4"/>
-      <c r="H96" s="4"/>
+      <c r="H96" s="11">
+        <v>2000</v>
+      </c>
       <c r="I96" s="4"/>
       <c r="J96" s="4"/>
       <c r="K96" s="4"/>

</xml_diff>

<commit_message>
data till 3Feb 8PM
</commit_message>
<xml_diff>
--- a/Daily Collection/February-2021-Collection.xlsx
+++ b/Daily Collection/February-2021-Collection.xlsx
@@ -577,10 +577,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="23">
@@ -600,66 +600,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -675,6 +615,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -684,10 +670,47 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -700,40 +723,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -788,7 +788,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -800,13 +842,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -818,19 +866,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -842,7 +884,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -854,7 +896,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -866,19 +914,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -890,7 +926,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -902,73 +962,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -979,6 +979,36 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1015,36 +1045,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1065,17 +1065,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1084,13 +1084,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1102,130 +1102,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1614,11 +1614,11 @@
   <dimension ref="A1:AO110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H96" sqref="H96"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1749,14 +1749,14 @@
       <c r="C2" s="7"/>
       <c r="D2" s="8">
         <f>SUM(F3:F121)</f>
-        <v>95900</v>
+        <v>128200</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="8">
         <f>SUM(G2:AK2)</f>
-        <v>95900</v>
+        <v>128200</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G121)</f>
@@ -1768,7 +1768,7 @@
       </c>
       <c r="I2" s="2">
         <f>SUM(I3:I121)</f>
-        <v>0</v>
+        <v>32300</v>
       </c>
       <c r="J2" s="2">
         <f>SUM(J3:J121)</f>
@@ -2002,13 +2002,15 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>2500</v>
+        <v>4500</v>
       </c>
       <c r="G5" s="4">
         <v>2500</v>
       </c>
       <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="I5" s="4">
+        <v>2000</v>
+      </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -2060,13 +2062,15 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="G6" s="11">
         <v>3000</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="I6" s="11">
+        <v>2000</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -2171,11 +2175,13 @@
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="I8" s="4">
+        <v>2000</v>
+      </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -2390,13 +2396,15 @@
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="4">
         <v>1500</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4">
+        <v>500</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -2501,7 +2509,7 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>6500</v>
+        <v>8500</v>
       </c>
       <c r="G14" s="4">
         <v>4500</v>
@@ -2509,7 +2517,9 @@
       <c r="H14" s="4">
         <v>2000</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4">
+        <v>2000</v>
+      </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -2617,13 +2627,15 @@
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
-        <v>1200</v>
+        <v>2200</v>
       </c>
       <c r="G16" s="11">
         <v>1200</v>
       </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="I16" s="4">
+        <v>1000</v>
+      </c>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -2953,13 +2965,15 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G22" s="4">
         <v>1000</v>
       </c>
       <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="I22" s="4">
+        <v>1000</v>
+      </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
@@ -3011,11 +3025,13 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="I23" s="4">
+        <v>3000</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -3177,11 +3193,13 @@
       </c>
       <c r="F26" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="I26" s="4">
+        <v>1500</v>
+      </c>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -3500,13 +3518,15 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G32" s="4">
         <v>1000</v>
       </c>
       <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
+      <c r="I32" s="4">
+        <v>1000</v>
+      </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -3552,11 +3572,13 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
+      <c r="I33" s="4">
+        <v>1000</v>
+      </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -3605,11 +3627,13 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
+      <c r="I34" s="4">
+        <v>1500</v>
+      </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -3760,11 +3784,13 @@
       </c>
       <c r="F37" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
+      <c r="I37" s="11">
+        <v>3000</v>
+      </c>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -4123,11 +4149,13 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
+      <c r="I44" s="4">
+        <v>3000</v>
+      </c>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -4395,11 +4423,13 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
+      <c r="I49" s="11">
+        <v>3000</v>
+      </c>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
@@ -4551,11 +4581,13 @@
       </c>
       <c r="F52" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
+      <c r="I52" s="11">
+        <v>1000</v>
+      </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -5341,11 +5373,13 @@
       </c>
       <c r="F67" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
+      <c r="I67" s="4">
+        <v>3000</v>
+      </c>
       <c r="J67" s="4"/>
       <c r="K67" s="4"/>
       <c r="L67" s="4"/>
@@ -5503,13 +5537,15 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" si="3"/>
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4">
         <v>1200</v>
       </c>
-      <c r="I70" s="4"/>
+      <c r="I70" s="4">
+        <v>800</v>
+      </c>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>

</xml_diff>

<commit_message>
data till 8Feb 8PM
</commit_message>
<xml_diff>
--- a/Daily Collection/February-2021-Collection.xlsx
+++ b/Daily Collection/February-2021-Collection.xlsx
@@ -578,8 +578,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
@@ -600,6 +600,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -614,9 +630,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -630,11 +654,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -647,10 +686,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -669,27 +708,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -701,30 +731,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -732,13 +739,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -788,13 +788,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,163 +968,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -982,17 +982,37 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1012,11 +1032,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1053,38 +1079,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1102,130 +1102,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1614,11 +1614,11 @@
   <dimension ref="A1:AO110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+      <selection pane="bottomRight" activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1749,14 +1749,14 @@
       <c r="C2" s="7"/>
       <c r="D2" s="8">
         <f>SUM(F3:F121)</f>
-        <v>259700</v>
+        <v>356800</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="8">
         <f>SUM(G2:AK2)</f>
-        <v>259700</v>
+        <v>356800</v>
       </c>
       <c r="G2" s="2">
         <f>SUM(G3:G121)</f>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="N2" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>97100</v>
       </c>
       <c r="O2" s="2">
         <f t="shared" si="0"/>
@@ -2002,7 +2002,7 @@
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
-        <v>6500</v>
+        <v>7500</v>
       </c>
       <c r="G5" s="4">
         <v>2500</v>
@@ -2017,7 +2017,9 @@
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="N5" s="4">
+        <v>1000</v>
+      </c>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
@@ -2064,7 +2066,7 @@
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="G6" s="11">
         <v>3000</v>
@@ -2077,7 +2079,9 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="N6" s="11">
+        <v>3000</v>
+      </c>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
@@ -2124,7 +2128,7 @@
       </c>
       <c r="F7" s="1">
         <f t="shared" si="1"/>
-        <v>8000</v>
+        <v>16000</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="11">
@@ -2137,7 +2141,9 @@
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
       <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="N7" s="11">
+        <v>8000</v>
+      </c>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
       <c r="Q7" s="4"/>
@@ -2463,7 +2469,7 @@
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>10000</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -2474,7 +2480,9 @@
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="N13" s="4">
+        <v>5000</v>
+      </c>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
       <c r="Q13" s="4"/>
@@ -2521,7 +2529,7 @@
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
-        <v>12500</v>
+        <v>16500</v>
       </c>
       <c r="G14" s="4">
         <v>4500</v>
@@ -2540,7 +2548,9 @@
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="N14" s="4">
+        <v>4000</v>
+      </c>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="4"/>
@@ -2585,7 +2595,7 @@
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="G15" s="4">
         <v>2000</v>
@@ -2596,7 +2606,9 @@
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
       <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="N15" s="4">
+        <v>2000</v>
+      </c>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
       <c r="Q15" s="4"/>
@@ -2703,7 +2715,7 @@
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4">
@@ -2714,7 +2726,9 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="N17" s="4">
+        <v>1000</v>
+      </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
       <c r="Q17" s="4"/>
@@ -2989,7 +3003,7 @@
       </c>
       <c r="F22" s="1">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="G22" s="4">
         <v>1000</v>
@@ -3002,7 +3016,9 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
+      <c r="N22" s="4">
+        <v>1000</v>
+      </c>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4"/>
@@ -3049,7 +3065,7 @@
       </c>
       <c r="F23" s="1">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
@@ -3062,7 +3078,9 @@
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="4"/>
-      <c r="N23" s="4"/>
+      <c r="N23" s="4">
+        <v>3000</v>
+      </c>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
       <c r="Q23" s="4"/>
@@ -3109,7 +3127,7 @@
       </c>
       <c r="F24" s="1">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="G24" s="11">
         <v>5000</v>
@@ -3122,7 +3140,9 @@
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
       <c r="M24" s="4"/>
-      <c r="N24" s="4"/>
+      <c r="N24" s="11">
+        <v>5000</v>
+      </c>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
       <c r="Q24" s="4"/>
@@ -3394,7 +3414,7 @@
       </c>
       <c r="F29" s="1">
         <f t="shared" si="1"/>
-        <v>5500</v>
+        <v>10500</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4">
@@ -3405,7 +3425,9 @@
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
       <c r="M29" s="4"/>
-      <c r="N29" s="4"/>
+      <c r="N29" s="4">
+        <v>5000</v>
+      </c>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
       <c r="Q29" s="4"/>
@@ -3501,7 +3523,7 @@
       </c>
       <c r="F31" s="1">
         <f t="shared" si="1"/>
-        <v>2500</v>
+        <v>4000</v>
       </c>
       <c r="G31" s="4">
         <v>1000</v>
@@ -3516,7 +3538,9 @@
         <v>500</v>
       </c>
       <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
+      <c r="N31" s="4">
+        <v>1500</v>
+      </c>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
@@ -3560,7 +3584,7 @@
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="G32" s="4">
         <v>1000</v>
@@ -3575,7 +3599,9 @@
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
       <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
+      <c r="N32" s="4">
+        <v>1000</v>
+      </c>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
       <c r="Q32" s="4"/>
@@ -3616,7 +3642,7 @@
       </c>
       <c r="F33" s="1">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
@@ -3627,7 +3653,9 @@
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
       <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
+      <c r="N33" s="4">
+        <v>1000</v>
+      </c>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
       <c r="Q33" s="4"/>
@@ -3671,7 +3699,7 @@
       </c>
       <c r="F34" s="1">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
@@ -3682,7 +3710,9 @@
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
       <c r="M34" s="4"/>
-      <c r="N34" s="4"/>
+      <c r="N34" s="4">
+        <v>2500</v>
+      </c>
       <c r="O34" s="4"/>
       <c r="P34" s="4"/>
       <c r="Q34" s="4"/>
@@ -3942,7 +3972,7 @@
       </c>
       <c r="F39" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -3951,7 +3981,9 @@
       <c r="K39" s="4"/>
       <c r="L39" s="4"/>
       <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
+      <c r="N39" s="4">
+        <v>4000</v>
+      </c>
       <c r="O39" s="4"/>
       <c r="P39" s="4"/>
       <c r="Q39" s="4"/>
@@ -4047,7 +4079,7 @@
       </c>
       <c r="F41" s="1">
         <f t="shared" si="2"/>
-        <v>7500</v>
+        <v>10500</v>
       </c>
       <c r="G41" s="4"/>
       <c r="H41" s="4">
@@ -4062,7 +4094,9 @@
       </c>
       <c r="L41" s="4"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
+      <c r="N41" s="4">
+        <v>3000</v>
+      </c>
       <c r="O41" s="4"/>
       <c r="P41" s="4"/>
       <c r="Q41" s="4"/>
@@ -4203,7 +4237,7 @@
       </c>
       <c r="F44" s="1">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -4214,7 +4248,9 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
+      <c r="N44" s="11">
+        <v>3000</v>
+      </c>
       <c r="O44" s="4"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
@@ -4312,7 +4348,7 @@
       </c>
       <c r="F46" s="1">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="G46" s="4"/>
       <c r="H46" s="4"/>
@@ -4325,7 +4361,9 @@
       </c>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
+      <c r="N46" s="4">
+        <v>3000</v>
+      </c>
       <c r="O46" s="4"/>
       <c r="P46" s="4"/>
       <c r="Q46" s="4"/>
@@ -4489,7 +4527,7 @@
       </c>
       <c r="F49" s="1">
         <f t="shared" si="2"/>
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -4502,7 +4540,9 @@
       <c r="K49" s="4"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
+      <c r="N49" s="4">
+        <v>3000</v>
+      </c>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
       <c r="Q49" s="4"/>
@@ -4870,7 +4910,7 @@
       </c>
       <c r="F56" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
@@ -4879,7 +4919,9 @@
       <c r="K56" s="4"/>
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
-      <c r="N56" s="4"/>
+      <c r="N56" s="11">
+        <v>15000</v>
+      </c>
       <c r="O56" s="4"/>
       <c r="P56" s="4"/>
       <c r="Q56" s="4"/>
@@ -4920,7 +4962,7 @@
       </c>
       <c r="F57" s="1">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="G57" s="4"/>
       <c r="H57" s="4">
@@ -4931,7 +4973,9 @@
       <c r="K57" s="4"/>
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
-      <c r="N57" s="4"/>
+      <c r="N57" s="4">
+        <v>2000</v>
+      </c>
       <c r="O57" s="4"/>
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
@@ -5036,7 +5080,7 @@
       </c>
       <c r="F59" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
@@ -5045,7 +5089,9 @@
       <c r="K59" s="4"/>
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
+      <c r="N59" s="11">
+        <v>5000</v>
+      </c>
       <c r="O59" s="4"/>
       <c r="P59" s="4"/>
       <c r="Q59" s="4"/>
@@ -5295,7 +5341,7 @@
       </c>
       <c r="F64" s="1">
         <f t="shared" si="2"/>
-        <v>1500</v>
+        <v>4000</v>
       </c>
       <c r="G64" s="4">
         <v>1500</v>
@@ -5306,7 +5352,9 @@
       <c r="K64" s="4"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
-      <c r="N64" s="4"/>
+      <c r="N64" s="4">
+        <v>2500</v>
+      </c>
       <c r="O64" s="4"/>
       <c r="P64" s="4"/>
       <c r="Q64" s="4"/>
@@ -5399,7 +5447,7 @@
       </c>
       <c r="F66" s="1">
         <f t="shared" si="2"/>
-        <v>10000</v>
+        <v>15000</v>
       </c>
       <c r="G66" s="4">
         <v>5000</v>
@@ -5412,7 +5460,9 @@
       <c r="K66" s="4"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
-      <c r="N66" s="4"/>
+      <c r="N66" s="4">
+        <v>5000</v>
+      </c>
       <c r="O66" s="4"/>
       <c r="P66" s="4"/>
       <c r="Q66" s="4"/>
@@ -5561,7 +5611,7 @@
       </c>
       <c r="F69" s="1">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
@@ -5572,7 +5622,9 @@
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4"/>
-      <c r="N69" s="4"/>
+      <c r="N69" s="4">
+        <v>1000</v>
+      </c>
       <c r="O69" s="4"/>
       <c r="P69" s="4"/>
       <c r="Q69" s="4"/>
@@ -5619,7 +5671,7 @@
       </c>
       <c r="F70" s="1">
         <f t="shared" si="3"/>
-        <v>3000</v>
+        <v>3600</v>
       </c>
       <c r="G70" s="4"/>
       <c r="H70" s="4">
@@ -5634,7 +5686,9 @@
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
+      <c r="N70" s="4">
+        <v>600</v>
+      </c>
       <c r="O70" s="4"/>
       <c r="P70" s="4"/>
       <c r="Q70" s="4"/>
@@ -5735,7 +5789,7 @@
       </c>
       <c r="F72" s="1">
         <f t="shared" si="3"/>
-        <v>5000</v>
+        <v>9000</v>
       </c>
       <c r="G72" s="4">
         <v>2000</v>
@@ -5750,7 +5804,9 @@
         <v>1500</v>
       </c>
       <c r="M72" s="4"/>
-      <c r="N72" s="4"/>
+      <c r="N72" s="4">
+        <v>4000</v>
+      </c>
       <c r="O72" s="4"/>
       <c r="P72" s="4"/>
       <c r="Q72" s="4"/>
@@ -6950,7 +7006,7 @@
       </c>
       <c r="F96" s="1">
         <f t="shared" si="3"/>
-        <v>2000</v>
+        <v>4000</v>
       </c>
       <c r="G96" s="4"/>
       <c r="H96" s="11">
@@ -6961,7 +7017,9 @@
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
       <c r="M96" s="4"/>
-      <c r="N96" s="4"/>
+      <c r="N96" s="11">
+        <v>2000</v>
+      </c>
       <c r="O96" s="4"/>
       <c r="P96" s="4"/>
       <c r="Q96" s="4"/>

</xml_diff>